<commit_message>
[CCORDERO] InceptionV3 62 classes results added
</commit_message>
<xml_diff>
--- a/presicion_analisis_InceptionV3.xlsx
+++ b/presicion_analisis_InceptionV3.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCE6DD8-7EDC-4509-A948-44ED03DB4F59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B53452-CECA-43BC-B5A3-8B1AF8B3EF9F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="4" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6InceptionV30.00004" sheetId="1" r:id="rId1"/>
     <sheet name="6InceptionV30.00008" sheetId="2" r:id="rId2"/>
     <sheet name="6InceptionV30.0001" sheetId="7" r:id="rId3"/>
     <sheet name="6InceptionV30.00007" sheetId="8" r:id="rId4"/>
-    <sheet name="6InceptionV30.00006" sheetId="9" r:id="rId5"/>
-    <sheet name="63InceptionV30.00006" sheetId="10" r:id="rId6"/>
+    <sheet name="63InceptionV30.00006" sheetId="10" r:id="rId5"/>
+    <sheet name="6InceptionV30.00006" sheetId="9" r:id="rId6"/>
     <sheet name="6InceptionV30.00006_ReduceLR" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -302,6 +302,99 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>475598</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66259</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70712D5D-B7DA-4D31-B814-D06D6A359623}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5219048" cy="3323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266074</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF4CFF2-BF24-4DA7-AF0C-58598665FB9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5534025" y="0"/>
+          <a:ext cx="5009524" cy="3400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>776449</xdr:colOff>
       <xdr:row>39</xdr:row>
@@ -330,55 +423,6 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="6323809" cy="7285714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>770933</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>126750</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF601589-FF05-42F4-8BEA-4FF91725FB8F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4733333" cy="7076190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -853,26 +897,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B24AC4-4AB1-47F9-B6C7-58411F0FECFF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7713032-E3C2-401B-9865-EB2A73AAF7D8}">
   <dimension ref="I10:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,11 +919,26 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B24AC4-4AB1-47F9-B6C7-58411F0FECFF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ADD32B-4F9D-4191-B08A-4888CD997953}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[CCORDERO] Xception no reduce added
</commit_message>
<xml_diff>
--- a/presicion_analisis_InceptionV3.xlsx
+++ b/presicion_analisis_InceptionV3.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B53452-CECA-43BC-B5A3-8B1AF8B3EF9F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492CE73E-C48B-42E3-BAC3-914302670577}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="4" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6InceptionV30.00004" sheetId="1" r:id="rId1"/>
     <sheet name="6InceptionV30.00008" sheetId="2" r:id="rId2"/>
     <sheet name="6InceptionV30.0001" sheetId="7" r:id="rId3"/>
     <sheet name="6InceptionV30.00007" sheetId="8" r:id="rId4"/>
-    <sheet name="63InceptionV30.00006" sheetId="10" r:id="rId5"/>
-    <sheet name="6InceptionV30.00006" sheetId="9" r:id="rId6"/>
-    <sheet name="6InceptionV30.00006_ReduceLR" sheetId="11" r:id="rId7"/>
+    <sheet name="6InceptionV30.00006" sheetId="9" r:id="rId5"/>
+    <sheet name="6InceptionV30.00006_ReduceLR" sheetId="11" r:id="rId6"/>
+    <sheet name="63InceptionV30.00006_ReduceLR" sheetId="10" r:id="rId7"/>
+    <sheet name="63InceptionV30.00006" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -293,6 +294,148 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>776449</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>153394</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EB305A7-307B-477F-97BA-D511F26D8A6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6323809" cy="7285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>772937</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>173013</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{245991BB-A9D7-4D27-B95F-B6FC5D970CC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3942857" cy="2733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142362</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B238E9-E9BC-4484-8819-A65C0B0ECE72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4754880" y="0"/>
+          <a:ext cx="4104762" cy="2752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -385,7 +528,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -395,17 +538,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>776449</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>153394</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>380458</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9139</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EB305A7-307B-477F-97BA-D511F26D8A6C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C9B4413-EC2C-47D3-B0A2-AAABE0ADCA39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -422,56 +565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6323809" cy="7285714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>772937</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>173013</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{245991BB-A9D7-4D27-B95F-B6FC5D970CC9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="3942857" cy="2733333"/>
+          <a:ext cx="4333333" cy="3085714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -489,16 +583,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>142362</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9181</xdr:rowOff>
+      <xdr:colOff>237601</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66282</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B238E9-E9BC-4484-8819-A65C0B0ECE72}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D1DB165-DF82-46F5-815B-F2D3E3AEFDD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -514,8 +608,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4754880" y="0"/>
-          <a:ext cx="4104762" cy="2752381"/>
+          <a:off x="4743450" y="0"/>
+          <a:ext cx="4190476" cy="3142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -897,10 +991,40 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B24AC4-4AB1-47F9-B6C7-58411F0FECFF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ADD32B-4F9D-4191-B08A-4888CD997953}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7713032-E3C2-401B-9865-EB2A73AAF7D8}">
   <dimension ref="I10:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -919,27 +1043,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B24AC4-4AB1-47F9-B6C7-58411F0FECFF}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F649F698-B9BC-4DD0-A506-B77112455116}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ADD32B-4F9D-4191-B08A-4888CD997953}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>